<commit_message>
Update Logbook Anton Ahlinder - ahan19tp.xlsx
</commit_message>
<xml_diff>
--- a/Logbooks/Logbook Anton Ahlinder - ahan19tp.xlsx
+++ b/Logbooks/Logbook Anton Ahlinder - ahan19tp.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myran\Desktop\Enchipsdatorer\IMS_Mower\Logbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5C59C8-7309-41DA-9BAF-83561B24F07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Work related to project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Initial meeting with project group</t>
+  </si>
+  <si>
+    <t>Brought home the robot, identified and studied the datasheets of the
+components</t>
+  </si>
+  <si>
+    <t>Meeting with the group, discussed work-structure and how to divide
+responsibilities</t>
+  </si>
+  <si>
+    <t>Bought adapter for micro-USB to USB-A as well as a SD-card reader. Both
+intended for use with the raspberry pi zero w.</t>
+  </si>
+  <si>
+    <t>Built the robot.</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week6</t>
+  </si>
+  <si>
+    <t>Conducted practical tests that confirmed that the code worked as intended.</t>
+  </si>
+  <si>
+    <t>Meeting with the other members working with the hardware. Discussed our 
+dependencies and how to tackle the different requirements of the project. Also demonstrated the code I had written and the autonomous movements of the robot.</t>
+  </si>
+  <si>
+    <t>Meeting with the entire project team. Presented our dependencies and
+discussed how to prioritize work going forward. Brief walkthrough of how 
+we should be using version control.</t>
+  </si>
+  <si>
+    <t>Wrote code for the functionality that makes the robot move autonomously inside a limited area. The area was limited by black tape which the robot is instructed to avoid. Also made the robot turn if it encountered an obstacle. Additionally, wrote code to gather data from the built in gyroscope on the robot. This could be used for the directional information that need to be sent to the backend.</t>
+  </si>
+  <si>
+    <t>Investigated different functions in the Makeblock library, specifically functions that make the engines turn a specified amount of degrees. This could be used to define the robots speed.</t>
+  </si>
+  <si>
+    <t>Found and shared an existing libray for Makeblock products. Many functions can be used for control of the robot.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,8 +144,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +445,323 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44648</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>44649</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>44650</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>44651</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44652</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>44653</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44654</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>44655</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>44656</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44657</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>44658</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>44659</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>44660</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>44661</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>44664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>44665</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>44666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>44667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>44668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>44670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>44671</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>44672</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>44674</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>44677</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>44678</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>44680</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>44682</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>44683</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>44686</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>44688</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>44689</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>